<commit_message>
added some data abd changed the scripting directory
</commit_message>
<xml_diff>
--- a/data/costs/afdb_costs.xlsx
+++ b/data/costs/afdb_costs.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghavpant/Desktop/git_projects/east-africa-transport/data/costs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A913734A-39B9-B347-80BE-F00BDB751E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389B52FA-7688-A246-938D-CE00329DA3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="620" windowWidth="19520" windowHeight="17280" xr2:uid="{D544D606-C289-6842-B5AC-CB27235F7C14}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="32180" windowHeight="18700" activeTab="2" xr2:uid="{D544D606-C289-6842-B5AC-CB27235F7C14}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="damage_costs_2006" sheetId="1" r:id="rId1"/>
+    <sheet name="damage_costs_2020" sheetId="3" r:id="rId2"/>
+    <sheet name="adaptation_costs_2006" sheetId="2" r:id="rId3"/>
+    <sheet name="adaptation_costs_2020" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>Type of road construction</t>
   </si>
@@ -58,19 +61,134 @@
   </si>
   <si>
     <t>&gt; 100 lane km</t>
+  </si>
+  <si>
+    <r>
+      <t>Type of road construction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Upgrading to paved road (US$/lane-km) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Periodic maintenance of paved roads (US$/lane-km)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>&lt; 100 lane km </t>
+  </si>
+  <si>
+    <t>Quartile 3 </t>
+  </si>
+  <si>
+    <t>Median </t>
+  </si>
+  <si>
+    <t>Quartile 1 </t>
+  </si>
+  <si>
+    <r>
+      <t>³</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> 100 lane km </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Regravelling of Unpaved roads (US$/lane-km)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rehabilitation of paved roads (US$/lane-km)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,9 +211,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,23 +534,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797C400B-2777-E648-9E00-B79C6ACE0148}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>290000</v>
+      </c>
+      <c r="E3" s="1">
+        <f>B3*(1+2.06/100)^(2020-2006)</f>
+        <v>13969.060394911232</v>
+      </c>
+      <c r="F3" s="1">
+        <f>C3*(1+2.06/100)^(2020-2006)</f>
+        <v>385812.14424040541</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9600</v>
+      </c>
+      <c r="C4" s="1">
+        <v>180300</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E9" si="0">B4*(1+2.06/100)^(2020-2006)</f>
+        <v>12771.712361061698</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F9" si="1">C4*(1+2.06/100)^(2020-2006)</f>
+        <v>239868.72278119001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8100</v>
+      </c>
+      <c r="C5" s="1">
+        <v>109800</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>10776.132304645807</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>146076.46012964315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12800</v>
+      </c>
+      <c r="C7" s="1">
+        <v>130500</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>17028.949814748928</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>173615.46490818245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11300</v>
+      </c>
+      <c r="C8" s="1">
+        <v>84400</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>15033.369758333039</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>112284.63784100076</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9600</v>
+      </c>
+      <c r="C9" s="1">
+        <v>47400</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>12771.712361061698</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>63060.329782742134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E89403-D988-4440-9D22-F231026F8391}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -439,10 +716,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>10500</v>
+        <v>13969.060394911232</v>
       </c>
       <c r="C3" s="1">
-        <v>290000</v>
+        <v>385812.14424040541</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -450,10 +727,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>9600</v>
+        <v>12771.712361061698</v>
       </c>
       <c r="C4" s="1">
-        <v>180300</v>
+        <v>239868.72278119001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -461,10 +738,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>8100</v>
+        <v>10776.132304645807</v>
       </c>
       <c r="C5" s="1">
-        <v>109800</v>
+        <v>146076.46012964315</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -477,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>12800</v>
+        <v>17028.949814748928</v>
       </c>
       <c r="C7" s="1">
-        <v>130500</v>
+        <v>173615.46490818245</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -488,10 +765,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>11300</v>
+        <v>15033.369758333039</v>
       </c>
       <c r="C8" s="1">
-        <v>84400</v>
+        <v>112284.63784100076</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -499,10 +776,232 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>9600</v>
+        <v>12771.712361061698</v>
       </c>
       <c r="C9" s="1">
-        <v>47400</v>
+        <v>63060.329782742134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DC01DD-A272-FA46-A985-94B69818D495}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
+        <v>425400</v>
+      </c>
+      <c r="C3" s="5">
+        <v>72200</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6">
+        <v>227800</v>
+      </c>
+      <c r="C4" s="5">
+        <v>64600</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>166300</v>
+      </c>
+      <c r="C5" s="5">
+        <v>56900</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
+        <v>162000</v>
+      </c>
+      <c r="C7" s="5">
+        <v>72200</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6">
+        <v>147100</v>
+      </c>
+      <c r="C8" s="5">
+        <v>64600</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <v>115900</v>
+      </c>
+      <c r="C9" s="5">
+        <v>56900</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33AE8A9-7B58-1A48-9526-D028712200EC}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
+        <v>461551.04814473714</v>
+      </c>
+      <c r="C3" s="5">
+        <v>78335.650390338546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6">
+        <v>247158.74181328423</v>
+      </c>
+      <c r="C4" s="5">
+        <v>70089.792454513445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>180432.39141154158</v>
+      </c>
+      <c r="C5" s="5">
+        <v>61735.436387953792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6">
+        <v>175766.9717899563</v>
+      </c>
+      <c r="C7" s="5">
+        <v>78335.650390338546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6">
+        <v>159600.7503105097</v>
+      </c>
+      <c r="C8" s="5">
+        <v>70089.792454513445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <v>125749.33352133294</v>
+      </c>
+      <c r="C9" s="5">
+        <v>61735.436387953792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>